<commit_message>
Added IE driver, updated datasheet and entered Step1 data from Excel
</commit_message>
<xml_diff>
--- a/SwissotelBooking/TestData/TestData.xlsx
+++ b/SwissotelBooking/TestData/TestData.xlsx
@@ -14,13 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
-  <si>
-    <t>Destination</t>
-  </si>
-  <si>
-    <t>Zurich, Swissotel</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>Title</t>
   </si>
@@ -92,13 +86,121 @@
   </si>
   <si>
     <t>VA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destination List </t>
+  </si>
+  <si>
+    <t>Field Name</t>
+  </si>
+  <si>
+    <t>Arrival Date (DD/MM/YYYY)</t>
+  </si>
+  <si>
+    <t>Departure Date (DD/MM/YYYY)</t>
+  </si>
+  <si>
+    <t>Booking Values</t>
+  </si>
+  <si>
+    <t>Modify Reservation values</t>
+  </si>
+  <si>
+    <t>Amsterdam, Netherlands</t>
+  </si>
+  <si>
+    <t>Ankara, Turkey</t>
+  </si>
+  <si>
+    <t>Bangkok, Thailand</t>
+  </si>
+  <si>
+    <t>Basel, Switzerland</t>
+  </si>
+  <si>
+    <t>Bodrum, Turkey</t>
+  </si>
+  <si>
+    <t>Chicago, United States</t>
+  </si>
+  <si>
+    <t>Dubai, United Arab Emirates</t>
+  </si>
+  <si>
+    <t>Foshan, China</t>
+  </si>
+  <si>
+    <t>Istanbul, Turkey</t>
+  </si>
+  <si>
+    <t>Izmir, Turkey</t>
+  </si>
+  <si>
+    <t>Kolkata, India</t>
+  </si>
+  <si>
+    <t>Kunshan, China</t>
+  </si>
+  <si>
+    <t>Lima, Peru</t>
+  </si>
+  <si>
+    <t>Makkah, Saudi Arabia</t>
+  </si>
+  <si>
+    <t>Moscow, Russia</t>
+  </si>
+  <si>
+    <t>Osaka, Japan</t>
+  </si>
+  <si>
+    <t>Phuket, Thailand</t>
+  </si>
+  <si>
+    <t>Quito, Ecuador</t>
+  </si>
+  <si>
+    <t>Sarajevo, Bosnia</t>
+  </si>
+  <si>
+    <t>Shanghai, China</t>
+  </si>
+  <si>
+    <t>Singapore, Singapore</t>
+  </si>
+  <si>
+    <t>Sochi, Russia</t>
+  </si>
+  <si>
+    <t>Sydney, Australia</t>
+  </si>
+  <si>
+    <t>Tallinn, Estonia</t>
+  </si>
+  <si>
+    <t>Zurich, Switzerland</t>
+  </si>
+  <si>
+    <t>Destination (Select from Drop down)</t>
+  </si>
+  <si>
+    <t>19/10/2019</t>
+  </si>
+  <si>
+    <t>25/10/2019</t>
+  </si>
+  <si>
+    <t>20/10/2019</t>
+  </si>
+  <si>
+    <t>26/10/2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,13 +208,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -142,16 +258,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,149 +573,293 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="K2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="K5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C6" s="2"/>
+      <c r="K6" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="K7" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2">
+        <v>20</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="K8" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1234567890</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="K9" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="K10" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="K11" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="K12" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="K13" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="K14" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2">
+        <v>123456</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="K15" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="K16" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C17" s="2"/>
+      <c r="K17" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2">
-        <v>1234567890</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="2">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C18" s="2"/>
+      <c r="K18" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="2">
+      <c r="B19" s="2">
         <v>2024</v>
       </c>
+      <c r="C19" s="2"/>
+      <c r="K19" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K22" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K24" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K25" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K26" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>$K$2:$K$26</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>